<commit_message>
Removed App and AppTest class Refactored code (to be readable :) ) Added all clases from maven project that needs to be inspected
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduard\Desktop\VVSS\Git\Docs\Lab01\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="156" windowWidth="14160" windowHeight="8268" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
     <sheet name="Architect. Design Phase Defects" sheetId="6" r:id="rId2"/>
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -76,12 +81,15 @@
   </si>
   <si>
     <t>Review Form. Requirements Defects</t>
+  </si>
+  <si>
+    <t>Onu Eduard Gabriel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -230,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -290,6 +298,9 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -299,6 +310,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -347,7 +361,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -382,7 +396,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -596,26 +610,26 @@
   </sheetPr>
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.3125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.89453125" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>19</v>
       </c>
@@ -623,7 +637,7 @@
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
@@ -632,7 +646,7 @@
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
@@ -641,22 +655,26 @@
       </c>
       <c r="E5" s="22"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="20" t="s">
+        <v>20</v>
+      </c>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="29">
+        <v>43542</v>
+      </c>
       <c r="E7" s="20"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -670,7 +688,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -678,7 +696,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -687,7 +705,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -696,7 +714,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -705,7 +723,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -714,7 +732,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -723,7 +741,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -732,7 +750,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -741,7 +759,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -750,7 +768,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -759,7 +777,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -768,7 +786,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="16"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -777,7 +795,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -786,7 +804,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="16"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -795,7 +813,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="16"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -804,7 +822,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="16"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -813,10 +831,10 @@
       <c r="D25" s="3"/>
       <c r="E25" s="16"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C27" s="12" t="s">
         <v>8</v>
       </c>
@@ -843,26 +861,26 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.3125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.89453125" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>18</v>
       </c>
@@ -870,7 +888,7 @@
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
@@ -879,7 +897,7 @@
       </c>
       <c r="E4" s="23"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
@@ -888,22 +906,26 @@
       </c>
       <c r="E5" s="25"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="20" t="s">
+        <v>20</v>
+      </c>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="29">
+        <v>43542</v>
+      </c>
       <c r="E7" s="20"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -917,7 +939,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -925,7 +947,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -934,7 +956,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -943,7 +965,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -952,7 +974,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -961,7 +983,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -970,7 +992,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -979,7 +1001,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -988,7 +1010,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -997,7 +1019,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1006,7 +1028,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1015,7 +1037,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1024,7 +1046,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1033,7 +1055,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1042,7 +1064,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1051,7 +1073,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1060,7 +1082,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1069,10 +1091,10 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C28" s="12" t="s">
         <v>8</v>
       </c>
@@ -1099,27 +1121,27 @@
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.3125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.89453125" style="6"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>17</v>
       </c>
@@ -1127,7 +1149,7 @@
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
@@ -1136,7 +1158,7 @@
       </c>
       <c r="E4" s="26"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
@@ -1145,22 +1167,26 @@
       </c>
       <c r="E5" s="28"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="20" t="s">
+        <v>20</v>
+      </c>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="29">
+        <v>43542</v>
+      </c>
       <c r="E7" s="20"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1174,7 +1200,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1182,7 +1208,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1191,7 +1217,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1200,7 +1226,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1209,7 +1235,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1218,7 +1244,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1227,7 +1253,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1236,7 +1262,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1245,7 +1271,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1254,7 +1280,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1263,7 +1289,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1272,7 +1298,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1281,7 +1307,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1290,7 +1316,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1299,7 +1325,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1308,7 +1334,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1317,7 +1343,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1326,7 +1352,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1335,7 +1361,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1344,7 +1370,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1353,7 +1379,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1362,10 +1388,10 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" s="12" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Finished requirements report. Finished modified requirements. Removed initial requiements.
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -84,19 +84,74 @@
   </si>
   <si>
     <t>Onu Eduard Gabriel</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>R03</t>
+  </si>
+  <si>
+    <t>R04</t>
+  </si>
+  <si>
+    <t>R05</t>
+  </si>
+  <si>
+    <t>R06</t>
+  </si>
+  <si>
+    <t>7(line)</t>
+  </si>
+  <si>
+    <t>La "adaugarea unei note la o materie" nu se specifica ce ar trebuie sa se intample daca apar cazuri exceptionale precum: nota nu este valida, nu exista un student cu numarul matricol introdus</t>
+  </si>
+  <si>
+    <t>9(line)</t>
+  </si>
+  <si>
+    <t>Nu se defineste exact cand un elev este "corigent". Acesta poate fi considerat corigent fie daca media sa este mai mica decat 5 fie mai mica decat 4.5.Acest lucru poate sa declaseaze ambiguitati si erori</t>
+  </si>
+  <si>
+    <t>8(line)</t>
+  </si>
+  <si>
+    <t>Daca un elev este corigent atunci nu trebuie sa I se mai calculeze media</t>
+  </si>
+  <si>
+    <t>NU</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Nu se specifica modul in care sunt stocate datele sunt stocate in fisierul text.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -238,69 +293,97 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,10 +691,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="N11" activeCellId="1" sqref="E16 N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,49 +713,49 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="19"/>
+      <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="22"/>
+      <c r="E5" s="21"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="20"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="22">
         <v>43542</v>
       </c>
-      <c r="E7" s="20"/>
+      <c r="E7" s="19"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -688,158 +771,201 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
+      <c r="C13" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="32" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
+      <c r="C14" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="32" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="31"/>
+      <c r="E15" s="32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="2"/>
+      <c r="C16" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="31"/>
+      <c r="E16" s="32" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="32"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="16"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="34"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="16"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="34"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="16"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="34"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="16"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="34"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="16"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="34"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="16"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="34"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="16"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="34"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="16"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="34"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E26" s="11"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="36"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="1"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C31" s="39" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -881,12 +1007,12 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
@@ -911,19 +1037,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="20"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="22">
         <v>43542</v>
       </c>
-      <c r="E7" s="20"/>
+      <c r="E7" s="19"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1142,15 +1268,15 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="26" t="s">
@@ -1159,7 +1285,7 @@
       <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="27" t="s">
@@ -1172,19 +1298,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="20"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="22">
         <v>43542</v>
       </c>
-      <c r="E7" s="20"/>
+      <c r="E7" s="19"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">

</xml_diff>

<commit_message>
Added report for arhitecture
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -132,6 +132,81 @@
   </si>
   <si>
     <t>Nu se specifica modul in care sunt stocate datele sunt stocate in fisierul text.</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>A04</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>A06</t>
+  </si>
+  <si>
+    <t>A07</t>
+  </si>
+  <si>
+    <t>A08</t>
+  </si>
+  <si>
+    <t>A09</t>
+  </si>
+  <si>
+    <t>repository/NoteRepositoryMock</t>
+  </si>
+  <si>
+    <t>Validarea unei note nu ar trebuie facuta intr-o metoda a acestei clase, ci intr-un validator, pentru a extinde scalabilitatea aplicatiei.</t>
+  </si>
+  <si>
+    <t>ClasaException</t>
+  </si>
+  <si>
+    <t>Aceasta clasa ar trebui sa fie in pachetul utils/exceptions nu in pachetul main.</t>
+  </si>
+  <si>
+    <t>Lipseste layer-ul servicii.Acest layer se ocupa cu logica aplicatiei.Aceasta logica a fost mutata in repository si de accea consider ca aplicatia nu a fost organizata bine pe layere.Lipsa validatori.</t>
+  </si>
+  <si>
+    <t>Nu putem calcula media unui student cu un anumit numar martricol.</t>
+  </si>
+  <si>
+    <t>repository</t>
+  </si>
+  <si>
+    <t>Clasele din acest pachet indeplinesc si alte functii diferite de cele pe care ar trebui sa le indeplineasca precum calculul de medie, sau afisarea unei clase.</t>
+  </si>
+  <si>
+    <t>Nu exista un mecanism bine definit pentru gesitunea erorilor.Nu se i-au in considerare cazurile exceptionale precum lipsa fisierului de elevi, si se omite tratarea erorii ClasaException</t>
+  </si>
+  <si>
+    <t>ClasaException, main</t>
+  </si>
+  <si>
+    <t>Nu, dar am putea adauga sabloane de proiectare, precum Singleton pentru controler/repository</t>
+  </si>
+  <si>
+    <t>ClasaException, Constants,ClasaRepositoryMock</t>
+  </si>
+  <si>
+    <t>Nu, in aceste 3 cazuri denumirile sunt prea generice.</t>
+  </si>
+  <si>
+    <t>ClasaRepositoryMock</t>
+  </si>
+  <si>
+    <t>Nu, deoarece un reposiotory nu ar trebui, sa incorporeze logica de calculare de medie si lucruri diferite inafara de operatiile CRUD.</t>
+  </si>
+  <si>
+    <t>A10</t>
   </si>
 </sst>
 </file>
@@ -293,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -317,6 +392,37 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -353,37 +459,9 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,7 +771,7 @@
   </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N11" activeCellId="1" sqref="E16 N11"/>
     </sheetView>
   </sheetViews>
@@ -713,49 +791,49 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="18"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="21"/>
+      <c r="E5" s="32"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="19"/>
+      <c r="E6" s="30"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="33">
         <v>43542</v>
       </c>
-      <c r="E7" s="19"/>
+      <c r="E7" s="30"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -775,13 +853,13 @@
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="18" t="s">
         <v>28</v>
       </c>
     </row>
@@ -790,13 +868,13 @@
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -805,13 +883,13 @@
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="18" t="s">
         <v>32</v>
       </c>
     </row>
@@ -820,11 +898,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="32" t="s">
+      <c r="D13" s="19"/>
+      <c r="E13" s="20" t="s">
         <v>33</v>
       </c>
     </row>
@@ -833,11 +911,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32" t="s">
+      <c r="D14" s="19"/>
+      <c r="E14" s="20" t="s">
         <v>33</v>
       </c>
     </row>
@@ -846,11 +924,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="32" t="s">
+      <c r="D15" s="19"/>
+      <c r="E15" s="20" t="s">
         <v>34</v>
       </c>
     </row>
@@ -859,11 +937,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="32" t="s">
+      <c r="D16" s="19"/>
+      <c r="E16" s="20" t="s">
         <v>36</v>
       </c>
     </row>
@@ -872,98 +950,98 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="32"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="34"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="34"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="34"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="22"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="34"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="22"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="34"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="22"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="34"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="22"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="34"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="22"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="34"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="22"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="36"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="24"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="38"/>
-      <c r="E27" s="31">
+      <c r="D27" s="26"/>
+      <c r="E27" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="39" t="s">
+      <c r="C31" s="27" t="s">
         <v>35</v>
       </c>
     </row>
@@ -987,8 +1065,8 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,49 +1085,49 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="36"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="19"/>
+      <c r="E6" s="30"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="33">
         <v>43542</v>
       </c>
-      <c r="E7" s="19"/>
+      <c r="E7" s="30"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1065,139 +1143,195 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="2"/>
+      <c r="C18" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="C19" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="2"/>
+      <c r="C20" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="2"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="18"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="2"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="18"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="2"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="18"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
@@ -1225,7 +1359,9 @@
         <v>8</v>
       </c>
       <c r="D28" s="13"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="40">
+        <v>6.25E-2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1268,49 +1404,49 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="26"/>
+      <c r="E4" s="37"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="28"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="19"/>
+      <c r="E6" s="30"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="33">
         <v>43542</v>
       </c>
-      <c r="E7" s="19"/>
+      <c r="E7" s="30"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">

</xml_diff>

<commit_message>
Finished report for code analysis
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="88">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -207,6 +207,84 @@
   </si>
   <si>
     <t>A10</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>C02</t>
+  </si>
+  <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>C04</t>
+  </si>
+  <si>
+    <t>C05</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>C07</t>
+  </si>
+  <si>
+    <t>C08</t>
+  </si>
+  <si>
+    <t>C09</t>
+  </si>
+  <si>
+    <t>if ( media &gt;= 4.5) trebuie transformat in if (media &lt; 4.5)</t>
+  </si>
+  <si>
+    <t>Corigent line 117</t>
+  </si>
+  <si>
+    <t>Corigent line 110</t>
+  </si>
+  <si>
+    <t>if(nrNote &gt;= 0) nu este necesar</t>
+  </si>
+  <si>
+    <t>Corigent line 101</t>
+  </si>
+  <si>
+    <t>if (clasa.size() &gt;= 0) nu este necesar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClasaRepositoryMock line 56 </t>
+  </si>
+  <si>
+    <t>if(clasa.size() &gt;= 0) trebuie transformat in if (clasa.size() &gt; 0) pentru a executa branch-ul pentru situatia in care clasa este goala</t>
+  </si>
+  <si>
+    <t>Nu</t>
+  </si>
+  <si>
+    <t>Da, daca nu exista fisierul pentru studenti/ note</t>
+  </si>
+  <si>
+    <t>main, linie 34</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>2 ore</t>
+  </si>
+  <si>
+    <t>1 ora si 30 minute</t>
+  </si>
+  <si>
+    <t>1 ora</t>
   </si>
 </sst>
 </file>
@@ -368,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -423,6 +501,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -459,8 +540,11 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -771,8 +855,8 @@
   </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" activeCellId="1" sqref="E16 N11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,49 +875,49 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="33"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="30"/>
+      <c r="E6" s="31"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="34">
         <v>43542</v>
       </c>
-      <c r="E7" s="30"/>
+      <c r="E7" s="31"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1036,8 +1120,8 @@
         <v>8</v>
       </c>
       <c r="D27" s="26"/>
-      <c r="E27" s="19">
-        <v>1</v>
+      <c r="E27" s="19" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
@@ -1065,8 +1149,8 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,49 +1169,49 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="35"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="37"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="30"/>
+      <c r="E6" s="31"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="34">
         <v>43542</v>
       </c>
-      <c r="E7" s="30"/>
+      <c r="E7" s="31"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1359,8 +1443,8 @@
         <v>8</v>
       </c>
       <c r="D28" s="13"/>
-      <c r="E28" s="40">
-        <v>6.25E-2</v>
+      <c r="E28" s="28" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1381,10 +1465,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,49 +1488,49 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="37"/>
+      <c r="E4" s="38"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="30"/>
+      <c r="E6" s="31"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="34">
         <v>43542</v>
       </c>
-      <c r="E7" s="30"/>
+      <c r="E7" s="31"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1462,203 +1546,274 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="C13" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="17"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="18"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="17"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="17"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="17"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E31" s="11"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="17"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="41"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C32" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="13"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Refactored all project Implemented exception handling Added packages: validators, interfaces, implementations, ui, serivce Added configuration class + maven dependencies Created validator for marks Removed logic for calculating avg for a student from repositoyClass Added NoteService Added UI Added MarkValidator Added Configuration Refactored report.xls
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="87">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -107,9 +107,6 @@
     <t>7(line)</t>
   </si>
   <si>
-    <t>La "adaugarea unei note la o materie" nu se specifica ce ar trebuie sa se intample daca apar cazuri exceptionale precum: nota nu este valida, nu exista un student cu numarul matricol introdus</t>
-  </si>
-  <si>
     <t>9(line)</t>
   </si>
   <si>
@@ -173,9 +170,6 @@
     <t>Aceasta clasa ar trebui sa fie in pachetul utils/exceptions nu in pachetul main.</t>
   </si>
   <si>
-    <t>Lipseste layer-ul servicii.Acest layer se ocupa cu logica aplicatiei.Aceasta logica a fost mutata in repository si de accea consider ca aplicatia nu a fost organizata bine pe layere.Lipsa validatori.</t>
-  </si>
-  <si>
     <t>Nu putem calcula media unui student cu un anumit numar martricol.</t>
   </si>
   <si>
@@ -245,15 +239,6 @@
     <t>Corigent line 110</t>
   </si>
   <si>
-    <t>if(nrNote &gt;= 0) nu este necesar</t>
-  </si>
-  <si>
-    <t>Corigent line 101</t>
-  </si>
-  <si>
-    <t>if (clasa.size() &gt;= 0) nu este necesar</t>
-  </si>
-  <si>
     <t xml:space="preserve">ClasaRepositoryMock line 56 </t>
   </si>
   <si>
@@ -285,6 +270,18 @@
   </si>
   <si>
     <t>1 ora</t>
+  </si>
+  <si>
+    <t>Lipseste layer-ul servicii.Acest layer se ocupa cu logica aplicatiei.Aceasta logica a fost mutata in repository si de accea consider ca aplicatia nu a fost organizata bine pe layere.Lipsa validatorilor, lipsa unui modul pentru configurari, lipsa unui obiect meniu.</t>
+  </si>
+  <si>
+    <t>if(nrNote &gt;= 0) trebuie transformat in if(nrNote &gt; 0)</t>
+  </si>
+  <si>
+    <t>Da, in cazul in care nu se dau in linia de comanda argumente</t>
+  </si>
+  <si>
+    <t>La "adaugarea unei note la o materie" nu se specifica ce ar trebuie sa se intample daca apar cazuri exceptionale precum: nota nu este valida, nu exista un student cu numarul matricol introdus, sau daca nota se va salva in fisier.</t>
   </si>
 </sst>
 </file>
@@ -504,6 +501,12 @@
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -539,12 +542,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -855,8 +852,8 @@
   </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,49 +872,49 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="35"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="33"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="36">
         <v>43542</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="33"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -933,7 +930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -944,7 +941,7 @@
         <v>27</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -956,10 +953,10 @@
         <v>22</v>
       </c>
       <c r="D11" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>29</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -971,10 +968,10 @@
         <v>23</v>
       </c>
       <c r="D12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>31</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -987,7 +984,7 @@
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1000,7 +997,7 @@
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1013,7 +1010,7 @@
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1026,7 +1023,7 @@
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -1121,12 +1118,12 @@
       </c>
       <c r="D27" s="26"/>
       <c r="E27" s="19" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C31" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1149,8 +1146,8 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,49 +1166,49 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="35"/>
+      <c r="E4" s="37"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="37"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="33"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="36">
         <v>43542</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="33"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1232,13 +1229,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="18" t="s">
         <v>46</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1247,26 +1244,26 @@
         <v>2</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="18" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1275,11 +1272,11 @@
         <v>4</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1288,13 +1285,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1303,13 +1300,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1318,11 +1315,11 @@
         <v>7</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="45" x14ac:dyDescent="0.25">
@@ -1331,13 +1328,13 @@
         <v>8</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="45" x14ac:dyDescent="0.25">
@@ -1346,13 +1343,13 @@
         <v>9</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -1361,11 +1358,11 @@
         <v>10</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -1374,11 +1371,11 @@
         <v>11</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -1444,7 +1441,7 @@
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="28" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1465,10 +1462,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1488,49 +1485,49 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="38"/>
+      <c r="E4" s="40"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="40"/>
+      <c r="E5" s="42"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="33"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="36">
         <v>43542</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="33"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1551,86 +1548,83 @@
         <v>1</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>3</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <f t="shared" ref="B13:B29" si="0">B12+1</f>
+        <v>4</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="18" t="s">
+      <c r="D13" s="18"/>
+      <c r="E13" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="3">
-        <f t="shared" ref="B12:B30" si="0">B11+1</f>
-        <v>3</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="17" t="s">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B13" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C14" s="17" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>81</v>
-      </c>
+      <c r="D15" s="18"/>
       <c r="E15" s="18" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1639,11 +1633,11 @@
         <v>7</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="18" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -1652,11 +1646,11 @@
         <v>8</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="18" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -1665,11 +1659,11 @@
         <v>9</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="D18" s="17"/>
       <c r="E18" s="18" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -1678,11 +1672,11 @@
         <v>10</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="17"/>
+        <v>68</v>
+      </c>
+      <c r="D19" s="18"/>
       <c r="E19" s="18" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -1691,11 +1685,11 @@
         <v>11</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="18"/>
+        <v>77</v>
+      </c>
+      <c r="D20" s="17"/>
       <c r="E20" s="18" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -1704,24 +1698,26 @@
         <v>12</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="17"/>
+        <v>78</v>
+      </c>
+      <c r="D21" s="18"/>
       <c r="E21" s="18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="3">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" s="18"/>
+      <c r="D22" s="18" t="s">
+        <v>76</v>
+      </c>
       <c r="E22" s="18" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
@@ -1729,13 +1725,9 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>84</v>
-      </c>
+      <c r="C23" s="17"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="18" t="s">
-        <v>79</v>
-      </c>
+      <c r="E23" s="18"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
@@ -1752,7 +1744,7 @@
         <v>16</v>
       </c>
       <c r="C25" s="17"/>
-      <c r="D25" s="18"/>
+      <c r="D25" s="17"/>
       <c r="E25" s="18"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -1761,8 +1753,8 @@
         <v>17</v>
       </c>
       <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="17"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
@@ -1771,7 +1763,7 @@
       </c>
       <c r="C27" s="17"/>
       <c r="D27" s="18"/>
-      <c r="E27" s="17"/>
+      <c r="E27" s="18"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
@@ -1792,28 +1784,19 @@
       <c r="E29" s="18"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="3">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="30"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="41"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="12" t="s">
+      <c r="C31" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="D31" s="13"/>
+      <c r="E31" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>